<commit_message>
Implementación de teclas de acceso rápido
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23325" windowHeight="7215"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -111,8 +112,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,11 +158,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,6 +241,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -269,6 +276,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,20 +452,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -465,15 +473,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -481,7 +492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -489,7 +500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -500,12 +511,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -513,7 +524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -521,12 +532,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -534,7 +545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -542,7 +553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -550,7 +561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -558,12 +569,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -571,7 +582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -579,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -587,17 +598,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -605,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -613,7 +624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -621,17 +632,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -643,12 +654,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -656,12 +667,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
actualización de planilla de avance.
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -148,10 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,8 +480,8 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
+      <c r="C2" s="3">
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,6 +491,9 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
+      <c r="C3" s="3">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -530,6 +533,9 @@
       </c>
       <c r="B8" t="s">
         <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actualizando planilla de progreso
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7215"/>
@@ -114,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -244,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -278,6 +279,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,20 +455,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -474,7 +476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -482,10 +484,10 @@
         <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -493,10 +495,10 @@
         <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -507,7 +509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -521,12 +523,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -534,7 +536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -545,12 +547,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -558,7 +560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -566,7 +568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -574,7 +576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -582,12 +584,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -595,7 +597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -603,7 +605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -614,17 +616,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -632,7 +634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -640,7 +642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -648,17 +650,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -670,12 +672,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -683,12 +685,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
actualización de status de planilla de progreso
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -459,7 +459,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,8 +543,8 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
+      <c r="C8">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,6 +641,9 @@
       <c r="B21" t="s">
         <v>21</v>
       </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -648,6 +651,9 @@
       </c>
       <c r="B22" t="s">
         <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Migracion de datos - quitando apellido y agregando actividad y razon social
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7215"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -109,14 +109,31 @@
   </si>
   <si>
     <t>Mas reportes se van a ir haciendo según necesidad con el sistema en uso</t>
+  </si>
+  <si>
+    <t>No, esta tarea la suprimimos porque es la opción de que un cliente modifique el pago de sus cuotas</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>Agregar patron fechas en todos los campos de fecha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,11 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,7 +189,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -244,7 +263,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +297,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,20 +472,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -476,7 +493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -487,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -498,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -509,7 +526,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -523,36 +540,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -560,36 +580,44 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -597,7 +625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -605,28 +633,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -634,7 +663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -645,7 +674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -656,19 +685,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -678,12 +715,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -691,12 +728,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Redondeo de cuotas sin decimal - actualizacion
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -552,8 +552,8 @@
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="C7" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">

</xml_diff>

<commit_message>
Cambios en tipos de dato fecha
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Agregar patron fechas en todos los campos de fecha</t>
+  </si>
+  <si>
+    <t>Falta en cuenta corriente - nueva cuota - ingreso de autorizacion</t>
+  </si>
+  <si>
+    <t>Validar fechas - permite cargar fechas q no existen</t>
+  </si>
+  <si>
+    <t>Lucas - ver como agregar validacion de fecha al fwk de validación que hiciste</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -503,6 +512,9 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -706,6 +718,14 @@
       </c>
       <c r="B26" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva tarea para fechas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -718,6 +718,9 @@
       </c>
       <c r="B26" t="s">
         <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:3">

</xml_diff>

<commit_message>
Actualizacion en Validaciones cliente
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Validar fechas - permite cargar fechas q no existen</t>
+  </si>
+  <si>
+    <t>AutorizationRequired anotacion en metodos privados, para poder validar antes</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -729,6 +732,14 @@
       </c>
       <c r="C27" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion de tarea completada
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>AutorizationRequired anotacion en metodos privados, para poder validar antes</t>
+  </si>
+  <si>
+    <t>Validacion de cuit para mostrar mensaje correcto</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -730,8 +733,8 @@
       <c r="B27" t="s">
         <v>22</v>
       </c>
-      <c r="C27" t="s">
-        <v>28</v>
+      <c r="C27" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -741,6 +744,14 @@
       <c r="B28" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificacion para permitir pagos parciales de cuotas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -488,7 +488,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -638,6 +638,9 @@
       </c>
       <c r="B15" t="s">
         <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">

</xml_diff>

<commit_message>
Actualziacion de pago parcial de cuotas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -488,7 +488,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -639,8 +639,8 @@
       <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">

</xml_diff>

<commit_message>
Actualizacion de tareas - nueva tarea
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Validacion de cuit para mostrar mensaje correcto</t>
+  </si>
+  <si>
+    <t>Validacion en creacion de cuota, no muestra los mensajes de error</t>
   </si>
 </sst>
 </file>
@@ -487,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -650,6 +653,9 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
@@ -754,7 +760,9 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizacion en pago de cuotas con un uncio comprobante por error en comprobante
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -653,8 +653,8 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
+      <c r="C16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">

</xml_diff>

<commit_message>
Actualizacion de estado de tareas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -628,7 +628,9 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Modificaciones en devolucion y estado de tareas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -803,8 +803,8 @@
       <c r="B31" t="s">
         <v>22</v>
       </c>
-      <c r="C31" t="s">
-        <v>28</v>
+      <c r="C31" s="3">
+        <v>0.7</v>
       </c>
     </row>
     <row r="32" spans="1:3">

</xml_diff>

<commit_message>
Modificacion en devoluciones y pagos con nota de credito
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7215"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -148,13 +148,16 @@
   </si>
   <si>
     <t>Borrar reportes del disco</t>
+  </si>
+  <si>
+    <t>ver cdo da error la venta igual genera las cuotas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,7 +222,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -293,7 +296,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -328,7 +330,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,20 +505,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -525,7 +526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -539,7 +540,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -550,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -561,7 +562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -575,12 +576,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -591,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -602,12 +603,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -615,7 +616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -624,7 +625,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -638,7 +639,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -649,7 +650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -660,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -671,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -682,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -693,18 +694,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -712,7 +713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -723,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -734,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -742,7 +743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -750,12 +751,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -766,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -777,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -788,17 +789,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -809,7 +810,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -820,15 +821,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -838,12 +844,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -851,12 +857,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificacion por error en cancelacion de cuota - modificacion en nota de credito
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>ver cdo da error la venta igual genera las cuotas</t>
+  </si>
+  <si>
+    <t>producto comodin</t>
+  </si>
+  <si>
+    <t>cambiar precio de producto</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -580,6 +586,12 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
@@ -712,6 +724,9 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
@@ -755,6 +770,9 @@
       <c r="A25" t="s">
         <v>29</v>
       </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
@@ -821,20 +839,36 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion por errores en devoluciones con nota de credito para pago de cuotas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>cambiar precio de producto</t>
+  </si>
+  <si>
+    <t>hacer configurable la ip de la printer</t>
+  </si>
+  <si>
+    <t>primer cuota - 1 mes mas</t>
+  </si>
+  <si>
+    <t>sacar cartel de cliente asociado con éxito</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -825,7 +834,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="3">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -869,6 +878,40 @@
     <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>46</v>
+      </c>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva tarea para lucas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>sacar cartel de cliente asociado con éxito</t>
+  </si>
+  <si>
+    <t>en venta - cdo pago con credito no muestra mensaje para avisar q modifique manualmente la nota y no esta validando si ya se uso un poco de guita</t>
+  </si>
+  <si>
+    <t>si pongo nota de credito inexistente no me da bola</t>
   </si>
 </sst>
 </file>
@@ -521,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -879,6 +885,9 @@
       <c r="A37" t="s">
         <v>46</v>
       </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3">
@@ -899,8 +908,8 @@
       <c r="B39" t="s">
         <v>22</v>
       </c>
-      <c r="C39" t="s">
-        <v>28</v>
+      <c r="C39" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -912,6 +921,16 @@
       </c>
       <c r="C40" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificacion en uso de nota de credito como medio de pago
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>sacar cartel de cliente asociado con éxito</t>
-  </si>
-  <si>
-    <t>en venta - cdo pago con credito no muestra mensaje para avisar q modifique manualmente la nota y no esta validando si ya se uso un poco de guita</t>
-  </si>
-  <si>
-    <t>si pongo nota de credito inexistente no me da bola</t>
   </si>
 </sst>
 </file>
@@ -527,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -921,16 +915,6 @@
       </c>
       <c r="C40" s="3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega producto comodin - no se debe actualizar el stock
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -524,7 +524,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -873,6 +873,12 @@
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">

</xml_diff>

<commit_message>
Se agrega producto comodin
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -765,6 +765,9 @@
       </c>
       <c r="B23" t="s">
         <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3">

</xml_diff>

<commit_message>
Se agrega talle a producto
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -766,8 +766,8 @@
       <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C23" t="s">
-        <v>28</v>
+      <c r="C23" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -777,6 +777,9 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
@@ -891,7 +894,9 @@
       <c r="B37" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">

</xml_diff>

<commit_message>
Se agrega reporte de zapatillas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Deshabilitar creacion de nueva cuota</t>
   </si>
   <si>
-    <t>vista detalle de cuota (venta asociada)</t>
-  </si>
-  <si>
     <t>Permitir pago parcial de cuotas</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>sacar cartel de cliente asociado con éxito</t>
+  </si>
+  <si>
+    <t>revisar reportes filtro fecha</t>
   </si>
 </sst>
 </file>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -535,10 +535,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -546,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -571,24 +571,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -596,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
         <v>0.8</v>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -634,7 +634,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -651,32 +651,32 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -687,7 +687,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -698,40 +698,40 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -742,18 +742,18 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>18</v>
+      <c r="A22" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -764,37 +764,37 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
+      <c r="A24" t="s">
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -815,21 +815,21 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -837,54 +837,54 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -892,10 +892,10 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -905,8 +905,8 @@
       <c r="B38" t="s">
         <v>21</v>
       </c>
-      <c r="C38" t="s">
-        <v>28</v>
+      <c r="C38" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -914,7 +914,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
@@ -923,12 +923,6 @@
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>49</v>
-      </c>
-      <c r="B40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se muestran los reportes sin guardarlos en el disco
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>AutorizationRequired anotacion en metodos privados, para poder validar antes</t>
-  </si>
-  <si>
-    <t>Validacion de cuit para mostrar mensaje correcto</t>
   </si>
   <si>
     <t>Validacion en creacion de cuota, no muestra los mensajes de error</t>
@@ -521,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -753,7 +750,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -815,13 +812,19 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -829,54 +832,60 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -886,7 +895,7 @@
       <c r="B36" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>27</v>
       </c>
     </row>
@@ -895,10 +904,10 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -915,17 +924,6 @@
     <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>48</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificacion en reportes y fechas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>acentos!</t>
+  </si>
+  <si>
+    <t>en los reportes faltan los decimales</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -628,6 +631,12 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -818,6 +827,12 @@
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
@@ -837,8 +852,8 @@
       <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C30" t="s">
-        <v>27</v>
+      <c r="C30" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -887,8 +902,8 @@
       <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>27</v>
+      <c r="C35" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -898,8 +913,8 @@
       <c r="B36" t="s">
         <v>20</v>
       </c>
-      <c r="C36" t="s">
-        <v>27</v>
+      <c r="C36" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -932,6 +947,17 @@
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se asigna revision estetica a Lucas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B34:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -860,7 +860,9 @@
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">

</xml_diff>

<commit_message>
Modificacion en etiqueta por acento
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B34:B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -717,7 +717,12 @@
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
@@ -863,6 +868,9 @@
       <c r="B31" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
@@ -949,6 +957,12 @@
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3">

</xml_diff>

<commit_message>
Creación de reporte de compra sugerida
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -723,8 +723,8 @@
       <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>27</v>
+      <c r="C17" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">

</xml_diff>

<commit_message>
Nueva tarea - reportes de devolucion
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Menu de pantalla principal y  botones (estetica)</t>
+  </si>
+  <si>
+    <t>revisar reportes de venta - devolucion</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -656,6 +659,9 @@
       <c r="B11" t="s">
         <v>22</v>
       </c>
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4">
@@ -982,6 +988,11 @@
     <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se quita requerimiento de autorizacion en algunos metodos
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>revisar reportes de venta - devolucion</t>
+  </si>
+  <si>
+    <t>Ivan: preguntar reportes - preguntar autorizacion requerida en que funciones - preguntar login</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -993,6 +996,11 @@
     <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Investigacion de reportes con graficos
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Ivan: preguntar reportes - preguntar autorizacion requerida en que funciones - preguntar login</t>
+  </si>
+  <si>
+    <t>http://mygnet.net/articulos/java/creacion_de_graficos_en_ireport.707</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -895,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
@@ -906,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -917,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -928,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -939,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -950,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -961,12 +964,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -977,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -988,17 +991,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Modificacion en patron de fechas para permitir blancos
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Reporte de stock minimo y de compra</t>
   </si>
   <si>
-    <t>Magic Button para borrar movimientos de stock</t>
-  </si>
-  <si>
     <t>Pedir a Ivan reportes control y estado para crearlos en el nuevo sistema</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>sacar cartel de cliente asociado con éxito</t>
   </si>
   <si>
-    <t>revisar reportes filtro fecha</t>
-  </si>
-  <si>
     <t>acentos!</t>
   </si>
   <si>
@@ -174,13 +168,49 @@
     <t>Menu de pantalla principal y  botones (estetica)</t>
   </si>
   <si>
-    <t>revisar reportes de venta - devolucion</t>
-  </si>
-  <si>
     <t>Ivan: preguntar reportes - preguntar autorizacion requerida en que funciones - preguntar login</t>
   </si>
   <si>
     <t>http://mygnet.net/articulos/java/creacion_de_graficos_en_ireport.707</t>
+  </si>
+  <si>
+    <t>lo que resta se hace manualmente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic Button para borrar movimientos de stock </t>
+  </si>
+  <si>
+    <t>Logo de susmann en blanco y negro - letras en negro para usar menos tinta</t>
+  </si>
+  <si>
+    <t>4593114 - telefono impresora</t>
+  </si>
+  <si>
+    <t>reporte movimiento cliente - los creditos van en haber</t>
+  </si>
+  <si>
+    <t>en stock agregar codigo - descripcion</t>
+  </si>
+  <si>
+    <t>reportes de venta diario (venta - devolucion) sin medios de pago</t>
+  </si>
+  <si>
+    <t>reportes de venta mensual (venta - devolucion) sin medios de pago</t>
+  </si>
+  <si>
+    <t>reportes de venta anual (venta - devolucion) sin medios de pago</t>
+  </si>
+  <si>
+    <t>rerportes venta de productos (agrupar por producto/tipo, con codigo y combo/marca)</t>
+  </si>
+  <si>
+    <t>reporte zapatillas - agregar marca en el reporte</t>
+  </si>
+  <si>
+    <t>movimientos de stock - agregar creacion</t>
+  </si>
+  <si>
+    <t>revisar todas las pantallas - patron fecha</t>
   </si>
 </sst>
 </file>
@@ -536,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -550,10 +580,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -561,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -575,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -586,24 +616,27 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -611,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
         <v>0.8</v>
@@ -622,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -633,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -644,7 +677,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -655,7 +688,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -663,10 +699,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -675,21 +711,21 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -700,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -711,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -722,7 +758,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -733,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -743,13 +779,19 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -760,18 +802,18 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>17</v>
+      <c r="A21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -782,18 +824,18 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
+      <c r="A23" t="s">
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -801,10 +843,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -812,10 +854,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
@@ -826,18 +868,18 @@
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -845,7 +887,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
@@ -859,32 +901,32 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -892,7 +934,7 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
@@ -903,20 +945,20 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="3">
+        <v>19</v>
+      </c>
+      <c r="C34" s="5">
         <v>1</v>
       </c>
     </row>
@@ -925,9 +967,9 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="5">
+        <v>19</v>
+      </c>
+      <c r="C35" s="3">
         <v>1</v>
       </c>
     </row>
@@ -947,7 +989,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -958,7 +1000,7 @@
         <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -968,6 +1010,12 @@
       <c r="A39" t="s">
         <v>47</v>
       </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
@@ -979,40 +1027,86 @@
       <c r="C40" s="3">
         <v>1</v>
       </c>
+      <c r="D40" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega funcionalidad para limpiar los movimientos de stock
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1038,8 +1038,8 @@
       <c r="B41" t="s">
         <v>20</v>
       </c>
-      <c r="C41" t="s">
-        <v>26</v>
+      <c r="C41" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1055,6 +1055,12 @@
     <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4">

</xml_diff>

<commit_message>
Modificacion en reporte de stock para ver marca
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -569,12 +569,12 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1051,6 +1051,12 @@
       <c r="A43" t="s">
         <v>56</v>
       </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
@@ -1059,8 +1065,8 @@
       <c r="B44" t="s">
         <v>20</v>
       </c>
-      <c r="C44" t="s">
-        <v>26</v>
+      <c r="C44" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">

</xml_diff>

<commit_message>
Modificacion de reporte de movimiento de clientes
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -647,7 +647,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1054,8 +1054,8 @@
       <c r="B43" t="s">
         <v>20</v>
       </c>
-      <c r="C43" t="s">
-        <v>26</v>
+      <c r="C43" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1072,6 +1072,12 @@
     <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:4">

</xml_diff>

<commit_message>
Actualizacion en reportes de venta (diario, mensual, anual)
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -201,9 +201,6 @@
     <t>reportes de venta anual (venta - devolucion) sin medios de pago</t>
   </si>
   <si>
-    <t>rerportes venta de productos (agrupar por producto/tipo, con codigo y combo/marca)</t>
-  </si>
-  <si>
     <t>reporte zapatillas - agregar marca en el reporte</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>revisar todas las pantallas - patron fecha</t>
+  </si>
+  <si>
+    <t>reportes venta de productos (agrupar por producto/tipo, con codigo y combo/marca)</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="B47" sqref="B47:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1076,33 +1076,45 @@
       <c r="B45" t="s">
         <v>20</v>
       </c>
-      <c r="C45" t="s">
-        <v>26</v>
+      <c r="C45" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>59</v>
       </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>60</v>
       </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -1113,7 +1125,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Modificacion en consulta de productos y stock (codigo)
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -569,7 +569,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:C47"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1106,10 +1106,22 @@
       <c r="A48" t="s">
         <v>64</v>
       </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:3">

</xml_diff>

<commit_message>
Se agregan las tareas del día - se arregla consulta de producto por codigo
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -211,6 +211,27 @@
   </si>
   <si>
     <t>reportes venta de productos (agrupar por producto/tipo, con codigo y combo/marca)</t>
+  </si>
+  <si>
+    <t>Estetica - botones imágenes</t>
+  </si>
+  <si>
+    <t>Estetica - etiquetas - tooltips - mensajes - mensajes de errores - etc</t>
+  </si>
+  <si>
+    <t>Logueo de aplicación (configurable)</t>
+  </si>
+  <si>
+    <t>Reportes - ruta - estitca</t>
+  </si>
+  <si>
+    <t>Reunion con Ivan y Josefina - consutlas</t>
+  </si>
+  <si>
+    <t>Impresora - carga de datos y factura</t>
+  </si>
+  <si>
+    <t>Lucas/Agustina</t>
   </si>
 </sst>
 </file>
@@ -567,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1147,8 +1168,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificaciones en reportes y en lista de tareas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>Lucas/Agustina</t>
+  </si>
+  <si>
+    <t>Agregar los comandos abajo, en la pantalla (teclas rapidas)</t>
+  </si>
+  <si>
+    <t>Agregar signo $ en los totales</t>
+  </si>
+  <si>
+    <t>En reportes mensual y anual poner mes y año, no dia!</t>
   </si>
 </sst>
 </file>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1193,6 +1202,7 @@
       <c r="B55" t="s">
         <v>19</v>
       </c>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
@@ -1210,8 +1220,29 @@
         <v>71</v>
       </c>
     </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificacion en venta por codigo de producto
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>En reportes mensual y anual poner mes y año, no dia!</t>
+  </si>
+  <si>
+    <t>No asignar cliente en venta de factura B</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1194,15 +1197,20 @@
       <c r="B54" t="s">
         <v>20</v>
       </c>
+      <c r="C54" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C55" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
@@ -1227,11 +1235,17 @@
       <c r="B58" t="s">
         <v>19</v>
       </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>73</v>
       </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
@@ -1239,6 +1253,14 @@
       </c>
       <c r="B60" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:1">

</xml_diff>

<commit_message>
Se agregan nuevas tareas
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Menu de pantalla principal y  botones (estetica)</t>
   </si>
   <si>
-    <t>Ivan: preguntar reportes - preguntar autorizacion requerida en que funciones - preguntar login</t>
-  </si>
-  <si>
     <t>http://mygnet.net/articulos/java/creacion_de_graficos_en_ireport.707</t>
   </si>
   <si>
@@ -244,6 +241,24 @@
   </si>
   <si>
     <t>No asignar cliente en venta de factura B</t>
+  </si>
+  <si>
+    <t>Error en iva cuando consumidor final en ticket</t>
+  </si>
+  <si>
+    <t>Error en listado de control - pagos de la fecha</t>
+  </si>
+  <si>
+    <t>Migracion de datos</t>
+  </si>
+  <si>
+    <t>Paginado de consultas</t>
+  </si>
+  <si>
+    <t>Reporte listado de cliente</t>
+  </si>
+  <si>
+    <t>Reporte para contador</t>
   </si>
 </sst>
 </file>
@@ -600,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -656,7 +671,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -725,7 +740,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1062,12 +1077,12 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
@@ -1078,12 +1093,12 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -1094,7 +1109,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -1105,7 +1120,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
@@ -1116,7 +1131,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
@@ -1127,7 +1142,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
@@ -1138,7 +1153,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
@@ -1149,7 +1164,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
@@ -1160,7 +1175,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -1171,7 +1186,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
@@ -1182,17 +1197,29 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
         <v>20</v>
@@ -1203,7 +1230,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
         <v>20</v>
@@ -1214,34 +1241,37 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
         <v>70</v>
-      </c>
-      <c r="B57" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
       </c>
-      <c r="C58" t="s">
-        <v>26</v>
+      <c r="C58" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
         <v>20</v>
@@ -1249,7 +1279,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
         <v>20</v>
@@ -1257,15 +1287,55 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>75</v>
       </c>
-      <c r="B61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva tarea para Lucasssssssss
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Reportes ingresos - ver con ivan que medios de pago sumar</t>
+  </si>
+  <si>
+    <t>Cuando no hay cliente asociado no setea en ventaDTO el campo tipoTicket</t>
   </si>
 </sst>
 </file>
@@ -618,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1347,6 +1350,14 @@
       </c>
       <c r="B68" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones por error en reporte de listado de control y en migracion de datos
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1317,6 +1317,9 @@
       <c r="B63" t="s">
         <v>20</v>
       </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
@@ -1325,26 +1328,32 @@
       <c r="B64" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>80</v>
       </c>
       <c r="B67" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Nuevas tareas para Lucas, que se ponga a laburar
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -24,9 +24,6 @@
     <t>validacion de usuario autorizador</t>
   </si>
   <si>
-    <t>proceso migración datos</t>
-  </si>
-  <si>
     <t>instalador</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>http://mygnet.net/articulos/java/creacion_de_graficos_en_ireport.707</t>
   </si>
   <si>
-    <t>lo que resta se hace manualmente</t>
-  </si>
-  <si>
     <t xml:space="preserve">Magic Button para borrar movimientos de stock </t>
   </si>
   <si>
@@ -265,6 +259,9 @@
   </si>
   <si>
     <t>Cuando no hay cliente asociado no setea en ventaDTO el campo tipoTicket</t>
+  </si>
+  <si>
+    <t>Setear corte z en el ticket</t>
   </si>
 </sst>
 </file>
@@ -623,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -635,10 +632,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -646,13 +643,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -660,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -668,30 +665,27 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -710,9 +704,9 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5">
         <v>1</v>
       </c>
     </row>
@@ -723,64 +717,64 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
+      <c r="D9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -791,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -802,31 +796,31 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="3">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -835,7 +829,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -846,18 +840,18 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>16</v>
+      <c r="A20" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -868,18 +862,18 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="6" t="s">
-        <v>24</v>
+      <c r="A22" t="s">
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -887,10 +881,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -898,10 +892,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -912,18 +906,18 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -931,7 +925,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -945,32 +939,32 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -978,7 +972,7 @@
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
@@ -989,20 +983,20 @@
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3">
+        <v>18</v>
+      </c>
+      <c r="C33" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1011,9 +1005,9 @@
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="5">
+        <v>18</v>
+      </c>
+      <c r="C34" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1033,7 +1027,7 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
@@ -1044,7 +1038,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -1066,48 +1060,54 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
       </c>
-      <c r="D40" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>52</v>
+      <c r="A41" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
@@ -1148,10 +1148,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
@@ -1159,10 +1159,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -1170,10 +1170,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C49" s="3">
         <v>1</v>
@@ -1181,10 +1181,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
@@ -1195,21 +1195,21 @@
         <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1217,7 +1217,7 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" s="3">
         <v>1</v>
@@ -1225,10 +1225,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" s="3">
         <v>1</v>
@@ -1239,7 +1239,7 @@
         <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C55" s="3">
         <v>1</v>
@@ -1247,13 +1247,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
         <v>68</v>
-      </c>
-      <c r="B56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1261,61 +1258,64 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>18</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
-      </c>
-      <c r="C58" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>74</v>
-      </c>
       <c r="B61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
@@ -1323,50 +1323,47 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="3">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B67" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B68" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>82</v>
-      </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrección de errores cuando no hay cliente asociado
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="7215"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15090" windowHeight="4605"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="82">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -267,8 +268,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,7 +335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -408,6 +409,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -442,6 +444,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -617,20 +620,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="77.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -638,7 +641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -652,7 +655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -663,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -677,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -688,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -699,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -710,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -721,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -732,7 +735,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -744,7 +747,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -758,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -769,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -780,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -791,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -802,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -813,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -824,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -835,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -846,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -857,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
@@ -868,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -879,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -890,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -901,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -912,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -923,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -934,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -945,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
@@ -956,7 +959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -967,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -978,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -989,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>51</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1291,15 +1294,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="C61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -1321,17 +1327,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1350,20 +1356,26 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B69" t="s">
         <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1373,12 +1385,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1386,12 +1398,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificaciones en estetica - botones e imagenes
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="15090" windowHeight="4605"/>
@@ -11,8 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -268,8 +267,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,7 +334,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -409,7 +408,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -444,7 +442,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,20 +617,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="77.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -641,7 +638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -655,7 +652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -666,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -680,7 +677,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -691,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -702,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -713,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -724,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -735,7 +732,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -747,7 +744,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -761,7 +758,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -772,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -783,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -794,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -805,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -816,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -827,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -838,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -849,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -860,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
@@ -871,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -882,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -893,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -904,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -915,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
@@ -926,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -937,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -948,18 +945,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>18</v>
+      <c r="B29" t="s">
+        <v>19</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -970,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -981,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
@@ -992,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1014,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1058,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1072,7 +1069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="6" t="s">
         <v>51</v>
       </c>
@@ -1094,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1127,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1138,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -1182,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1193,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1204,7 +1201,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -1215,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1237,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1248,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -1267,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -1275,7 +1272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1294,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -1316,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -1327,17 +1324,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -1348,7 +1345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1356,7 +1353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>80</v>
       </c>
@@ -1367,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>81</v>
       </c>
@@ -1385,12 +1382,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1398,12 +1395,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificaciones en manejo de excepciones
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Setear corte z en el ticket</t>
+  </si>
+  <si>
+    <t>Intro en ventana para crear cuota</t>
   </si>
 </sst>
 </file>
@@ -618,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1198,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="C51" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1373,6 +1376,14 @@
       </c>
       <c r="C69" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion en Manejo de errores - actualizacion de reporte de contador
</commit_message>
<xml_diff>
--- a/mitnick.xlsx
+++ b/mitnick.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>teclas acceso rapido</t>
   </si>
@@ -93,9 +93,6 @@
     <t>reportes - estética para imprimir y mostrar a Ivan</t>
   </si>
   <si>
-    <t>en proceso</t>
-  </si>
-  <si>
     <t>modificar reportes de venta para contemplar flag cancelado</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>Intro en ventana para crear cuota</t>
+  </si>
+  <si>
+    <t>mensaje de confirmacion de cierre z</t>
   </si>
 </sst>
 </file>
@@ -621,9 +621,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -732,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -755,10 +755,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -854,7 +854,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -961,7 +961,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
@@ -972,10 +972,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -1069,12 +1069,12 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
@@ -1239,10 +1239,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="3">
         <v>1</v>
@@ -1250,15 +1250,15 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
         <v>67</v>
-      </c>
-      <c r="B56" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
@@ -1269,34 +1269,28 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B60" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
@@ -1307,7 +1301,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
@@ -1329,62 +1323,73 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
-      <c r="C66" t="s">
-        <v>25</v>
+      <c r="C66" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B67" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="2" t="s">
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B68" t="s">
-        <v>18</v>
-      </c>
-      <c r="C68" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="B69" t="s">
         <v>18</v>
       </c>
-      <c r="C69" t="s">
-        <v>25</v>
+      <c r="C69" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>82</v>
       </c>
-      <c r="B70" t="s">
-        <v>18</v>
-      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>